<commit_message>
added some func to Adc.
</commit_message>
<xml_diff>
--- a/misc/LCR calc.xlsx
+++ b/misc/LCR calc.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekty\reszta\LCRmeter\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05B83887-47F4-4B3A-AF00-5F0DBFA42B78}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72BE98FF-5B02-4B32-A13A-D3E2DF7DB3CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="8040" xr2:uid="{E87E0838-13C8-43A6-B33A-F14C82948CED}"/>
+    <workbookView xWindow="-19320" yWindow="600" windowWidth="19440" windowHeight="15150" xr2:uid="{E87E0838-13C8-43A6-B33A-F14C82948CED}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,6 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="14">
   <si>
     <t>rad</t>
   </si>
@@ -51,6 +52,27 @@
   </si>
   <si>
     <t>,</t>
+  </si>
+  <si>
+    <t>12Mhz</t>
+  </si>
+  <si>
+    <t>PI</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>Sine table</t>
+  </si>
+  <si>
+    <t>9Mhz</t>
+  </si>
+  <si>
+    <t>ADC sampling time in microseconds, based on clock cycles. (Fcpu=72mhz)</t>
+  </si>
+  <si>
+    <t>DO NOT USE THIS AS 100% CORRECT SOURCE</t>
   </si>
 </sst>
 </file>
@@ -75,7 +97,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -83,12 +105,107 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -403,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14015742-D441-4FFB-89F0-A5D4498946AF}">
-  <dimension ref="A1:K259"/>
+  <dimension ref="A1:J259"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J259" sqref="I4:J259"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -414,19 +531,28 @@
     <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="77.5703125" customWidth="1"/>
     <col min="3" max="3" width="24.7109375" customWidth="1"/>
+    <col min="5" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B1">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="3"/>
+      <c r="B1" s="4">
         <f>PI()/2-(A4+ASIN(A6*SIN(A4)/A8))</f>
         <v>2.8566562920418002</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B2">
+      <c r="C1" s="5"/>
+      <c r="H1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="6"/>
+      <c r="B2" s="7">
         <f>DEGREES(B1)</f>
         <v>163.67434905348628</v>
       </c>
+      <c r="C2" s="8"/>
       <c r="H2">
         <v>256</v>
       </c>
@@ -435,20 +561,29 @@
         <v>2.4543692606170259E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="7">
         <f>PI()-B1</f>
         <v>0.28493636154799296</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="C3" s="8"/>
+      <c r="H3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
         <f>RADIANS(-39.92)</f>
         <v>-0.69673543739613641</v>
       </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="8"/>
       <c r="H4">
         <f>I2</f>
         <v>2.4543692606170259E-2</v>
@@ -460,16 +595,13 @@
       <c r="J4" t="s">
         <v>6</v>
       </c>
-      <c r="K4">
-        <f>I4</f>
-        <v>129</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C5" t="s">
+      <c r="B5" s="7"/>
+      <c r="C5" s="8" t="s">
         <v>3</v>
       </c>
       <c r="H5">
@@ -484,11 +616,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
         <v>0.99399999999999999</v>
       </c>
-      <c r="C6">
+      <c r="B6" s="7"/>
+      <c r="C6" s="8">
         <f>0.994*COS(B3)</f>
         <v>0.95392146588028093</v>
       </c>
@@ -504,10 +637,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>2</v>
       </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
       <c r="H7">
         <f t="shared" si="1"/>
         <v>9.8174770424681035E-2</v>
@@ -520,10 +661,16 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
         <v>1.1479999999999999</v>
       </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
       <c r="H8">
         <f t="shared" si="1"/>
         <v>0.12271846303085129</v>
@@ -536,7 +683,16 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
       <c r="H9">
         <f t="shared" si="1"/>
         <v>0.14726215563702155</v>
@@ -549,7 +705,25 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="6"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10">
+        <v>1.5</v>
+      </c>
+      <c r="E10">
+        <f>1/12000000*(D10+12.5)</f>
+        <v>1.1666666666666668E-6</v>
+      </c>
+      <c r="F10">
+        <f>ROUND(E10,9)</f>
+        <v>1.167E-6</v>
+      </c>
+      <c r="G10">
+        <f>F10*1000000</f>
+        <v>1.167</v>
+      </c>
       <c r="H10">
         <f t="shared" si="1"/>
         <v>0.17180584824319181</v>
@@ -562,10 +736,27 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
         <v>0</v>
       </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="8"/>
+      <c r="D11">
+        <v>7.5</v>
+      </c>
+      <c r="E11">
+        <f t="shared" ref="E11:E17" si="2">1/12000000*(D11+12.5)</f>
+        <v>1.6666666666666667E-6</v>
+      </c>
+      <c r="F11">
+        <f t="shared" ref="F11:F25" si="3">ROUND(E11,9)</f>
+        <v>1.6670000000000001E-6</v>
+      </c>
+      <c r="G11">
+        <f t="shared" ref="G11:G25" si="4">F11*1000000</f>
+        <v>1.667</v>
+      </c>
       <c r="H11">
         <f t="shared" si="1"/>
         <v>0.19634954084936207</v>
@@ -578,11 +769,28 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
         <f>RADIANS(33.18)</f>
         <v>0.57910024581171848</v>
       </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="8"/>
+      <c r="D12">
+        <v>13.5</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="2"/>
+        <v>2.166666666666667E-6</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="3"/>
+        <v>2.1670000000000002E-6</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="4"/>
+        <v>2.1670000000000003</v>
+      </c>
       <c r="H12">
         <f t="shared" si="1"/>
         <v>0.22089323345553233</v>
@@ -595,13 +803,29 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="7" t="s">
         <v>4</v>
       </c>
+      <c r="C13" s="8"/>
+      <c r="D13">
+        <v>28.5</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="2"/>
+        <v>3.4166666666666668E-6</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="3"/>
+        <v>3.4170000000000001E-6</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="4"/>
+        <v>3.4170000000000003</v>
+      </c>
       <c r="H13">
         <f t="shared" si="1"/>
         <v>0.24543692606170259</v>
@@ -614,14 +838,30 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
         <v>0.29099999999999998</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="7">
         <f>PI()/2-(A12+ACOS((A18-A14*COS(A12))/A16))</f>
         <v>0.25110222169560625</v>
       </c>
+      <c r="C14" s="8"/>
+      <c r="D14">
+        <v>41.5</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="2"/>
+        <v>4.5000000000000001E-6</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="3"/>
+        <v>4.5000000000000001E-6</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="4"/>
+        <v>4.5</v>
+      </c>
       <c r="H14">
         <f t="shared" si="1"/>
         <v>0.26998061866787282</v>
@@ -634,14 +874,30 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="7">
         <f>DEGREES(B14)</f>
         <v>14.387097529516572</v>
       </c>
+      <c r="C15" s="8"/>
+      <c r="D15">
+        <v>55.5</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="2"/>
+        <v>5.6666666666666669E-6</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="3"/>
+        <v>5.6670000000000001E-6</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="4"/>
+        <v>5.6669999999999998</v>
+      </c>
       <c r="H15">
         <f t="shared" si="1"/>
         <v>0.2945243112740431</v>
@@ -654,14 +910,30 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
         <v>0.23499999999999999</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="7">
         <f>PI()-B14</f>
         <v>2.8904904318941869</v>
       </c>
+      <c r="C16" s="8"/>
+      <c r="D16">
+        <v>71.5</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="2"/>
+        <v>7.0000000000000007E-6</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="3"/>
+        <v>6.9999999999999999E-6</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
       <c r="H16">
         <f t="shared" si="1"/>
         <v>0.31906800388021339</v>
@@ -675,9 +947,26 @@
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="6" t="s">
         <v>5</v>
       </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="8"/>
+      <c r="D17">
+        <v>239.5</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="2"/>
+        <v>2.1000000000000002E-5</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="3"/>
+        <v>2.0999999999999999E-5</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="4"/>
+        <v>21</v>
+      </c>
       <c r="H17">
         <f t="shared" si="1"/>
         <v>0.34361169648638368</v>
@@ -691,9 +980,11 @@
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="A18" s="6">
         <v>0.41699999999999998</v>
       </c>
+      <c r="B18" s="7"/>
+      <c r="C18" s="8"/>
       <c r="H18">
         <f t="shared" si="1"/>
         <v>0.36815538909255396</v>
@@ -707,6 +998,15 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="9"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
       <c r="H19">
         <f t="shared" si="1"/>
         <v>0.39269908169872425</v>
@@ -720,6 +1020,21 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <v>1.5</v>
+      </c>
+      <c r="E20">
+        <f>1/9000000*(D20+12.5)</f>
+        <v>1.5555555555555556E-6</v>
+      </c>
+      <c r="F20">
+        <f>ROUND(E20,9)</f>
+        <v>1.556E-6</v>
+      </c>
+      <c r="G20">
+        <f>F20*1000000</f>
+        <v>1.556</v>
+      </c>
       <c r="H20">
         <f t="shared" si="1"/>
         <v>0.41724277430489454</v>
@@ -733,6 +1048,24 @@
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21">
+        <v>7.5</v>
+      </c>
+      <c r="E21">
+        <f t="shared" ref="E21:E27" si="5">1/9000000*(D21+12.5)</f>
+        <v>2.2222222222222221E-6</v>
+      </c>
+      <c r="F21">
+        <f>ROUND(E21,9)</f>
+        <v>2.2220000000000001E-6</v>
+      </c>
+      <c r="G21">
+        <f>F21*1000000</f>
+        <v>2.222</v>
+      </c>
       <c r="H21">
         <f t="shared" si="1"/>
         <v>0.44178646691106482</v>
@@ -746,6 +1079,21 @@
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <v>13.5</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="5"/>
+        <v>2.888888888888889E-6</v>
+      </c>
+      <c r="F22">
+        <f>ROUND(E22,9)</f>
+        <v>2.8890000000000002E-6</v>
+      </c>
+      <c r="G22">
+        <f>F22*1000000</f>
+        <v>2.8890000000000002</v>
+      </c>
       <c r="H22">
         <f t="shared" si="1"/>
         <v>0.46633015951723511</v>
@@ -759,6 +1107,21 @@
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D23">
+        <v>28.5</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="5"/>
+        <v>4.5555555555555552E-6</v>
+      </c>
+      <c r="F23">
+        <f>ROUND(E23,9)</f>
+        <v>4.5560000000000001E-6</v>
+      </c>
+      <c r="G23">
+        <f>F23*1000000</f>
+        <v>4.556</v>
+      </c>
       <c r="H23">
         <f t="shared" si="1"/>
         <v>0.4908738521234054</v>
@@ -772,6 +1135,21 @@
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D24">
+        <v>41.5</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="5"/>
+        <v>6.0000000000000002E-6</v>
+      </c>
+      <c r="F24">
+        <f>ROUND(E24,9)</f>
+        <v>6.0000000000000002E-6</v>
+      </c>
+      <c r="G24">
+        <f>F24*1000000</f>
+        <v>6</v>
+      </c>
       <c r="H24">
         <f t="shared" si="1"/>
         <v>0.51541754472957568</v>
@@ -785,6 +1163,21 @@
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D25">
+        <v>55.5</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="5"/>
+        <v>7.5555555555555553E-6</v>
+      </c>
+      <c r="F25">
+        <f>ROUND(E25,9)</f>
+        <v>7.5560000000000002E-6</v>
+      </c>
+      <c r="G25">
+        <f>F25*1000000</f>
+        <v>7.556</v>
+      </c>
       <c r="H25">
         <f t="shared" si="1"/>
         <v>0.53996123733574597</v>
@@ -798,6 +1191,21 @@
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D26">
+        <v>71.5</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="5"/>
+        <v>9.3333333333333326E-6</v>
+      </c>
+      <c r="F26">
+        <f>ROUND(E26,9)</f>
+        <v>9.3330000000000003E-6</v>
+      </c>
+      <c r="G26">
+        <f>F26*1000000</f>
+        <v>9.3330000000000002</v>
+      </c>
       <c r="H26">
         <f t="shared" si="1"/>
         <v>0.56450492994191626</v>
@@ -811,6 +1219,21 @@
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D27">
+        <v>239.5</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="5"/>
+        <v>2.8E-5</v>
+      </c>
+      <c r="F27">
+        <f>ROUND(E27,9)</f>
+        <v>2.8E-5</v>
+      </c>
+      <c r="G27">
+        <f>F27*1000000</f>
+        <v>28</v>
+      </c>
       <c r="H27">
         <f t="shared" si="1"/>
         <v>0.58904862254808654</v>
@@ -1362,7 +1785,7 @@
         <v>1.6198837120072358</v>
       </c>
       <c r="I69">
-        <f t="shared" ref="I69:I132" si="2">ROUND(SIN(H69)*64+127,0)</f>
+        <f t="shared" ref="I69:I132" si="6">ROUND(SIN(H69)*64+127,0)</f>
         <v>191</v>
       </c>
       <c r="J69" t="s">
@@ -1371,11 +1794,11 @@
     </row>
     <row r="70" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H70">
-        <f t="shared" ref="H70:H133" si="3">H69+$I$2</f>
+        <f t="shared" ref="H70:H133" si="7">H69+$I$2</f>
         <v>1.644427404613406</v>
       </c>
       <c r="I70">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>191</v>
       </c>
       <c r="J70" t="s">
@@ -1384,11 +1807,11 @@
     </row>
     <row r="71" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H71">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1.6689710972195761</v>
       </c>
       <c r="I71">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>191</v>
       </c>
       <c r="J71" t="s">
@@ -1397,11 +1820,11 @@
     </row>
     <row r="72" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H72">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1.6935147898257463</v>
       </c>
       <c r="I72">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>191</v>
       </c>
       <c r="J72" t="s">
@@ -1410,11 +1833,11 @@
     </row>
     <row r="73" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H73">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1.7180584824319165</v>
       </c>
       <c r="I73">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>190</v>
       </c>
       <c r="J73" t="s">
@@ -1423,11 +1846,11 @@
     </row>
     <row r="74" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H74">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1.7426021750380867</v>
       </c>
       <c r="I74">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>190</v>
       </c>
       <c r="J74" t="s">
@@ -1436,11 +1859,11 @@
     </row>
     <row r="75" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H75">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1.7671458676442569</v>
       </c>
       <c r="I75">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>190</v>
       </c>
       <c r="J75" t="s">
@@ -1449,11 +1872,11 @@
     </row>
     <row r="76" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H76">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1.791689560250427</v>
       </c>
       <c r="I76">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>189</v>
       </c>
       <c r="J76" t="s">
@@ -1462,11 +1885,11 @@
     </row>
     <row r="77" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H77">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1.8162332528565972</v>
       </c>
       <c r="I77">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>189</v>
       </c>
       <c r="J77" t="s">
@@ -1475,11 +1898,11 @@
     </row>
     <row r="78" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H78">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1.8407769454627674</v>
       </c>
       <c r="I78">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>189</v>
       </c>
       <c r="J78" t="s">
@@ -1488,11 +1911,11 @@
     </row>
     <row r="79" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H79">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1.8653206380689376</v>
       </c>
       <c r="I79">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>188</v>
       </c>
       <c r="J79" t="s">
@@ -1501,11 +1924,11 @@
     </row>
     <row r="80" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H80">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1.8898643306751077</v>
       </c>
       <c r="I80">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>188</v>
       </c>
       <c r="J80" t="s">
@@ -1514,11 +1937,11 @@
     </row>
     <row r="81" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1.9144080232812779</v>
       </c>
       <c r="I81">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>187</v>
       </c>
       <c r="J81" t="s">
@@ -1527,11 +1950,11 @@
     </row>
     <row r="82" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H82">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1.9389517158874481</v>
       </c>
       <c r="I82">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>187</v>
       </c>
       <c r="J82" t="s">
@@ -1540,11 +1963,11 @@
     </row>
     <row r="83" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H83">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1.9634954084936183</v>
       </c>
       <c r="I83">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>186</v>
       </c>
       <c r="J83" t="s">
@@ -1553,11 +1976,11 @@
     </row>
     <row r="84" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H84">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1.9880391010997884</v>
       </c>
       <c r="I84">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>186</v>
       </c>
       <c r="J84" t="s">
@@ -1566,11 +1989,11 @@
     </row>
     <row r="85" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H85">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2.0125827937059588</v>
       </c>
       <c r="I85">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>185</v>
       </c>
       <c r="J85" t="s">
@@ -1579,11 +2002,11 @@
     </row>
     <row r="86" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H86">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2.037126486312129</v>
       </c>
       <c r="I86">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>184</v>
       </c>
       <c r="J86" t="s">
@@ -1592,11 +2015,11 @@
     </row>
     <row r="87" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H87">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2.0616701789182992</v>
       </c>
       <c r="I87">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>183</v>
       </c>
       <c r="J87" t="s">
@@ -1605,11 +2028,11 @@
     </row>
     <row r="88" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H88">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2.0862138715244694</v>
       </c>
       <c r="I88">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>183</v>
       </c>
       <c r="J88" t="s">
@@ -1618,11 +2041,11 @@
     </row>
     <row r="89" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H89">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2.1107575641306395</v>
       </c>
       <c r="I89">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>182</v>
       </c>
       <c r="J89" t="s">
@@ -1631,11 +2054,11 @@
     </row>
     <row r="90" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H90">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2.1353012567368097</v>
       </c>
       <c r="I90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>181</v>
       </c>
       <c r="J90" t="s">
@@ -1644,11 +2067,11 @@
     </row>
     <row r="91" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H91">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2.1598449493429799</v>
       </c>
       <c r="I91">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>180</v>
       </c>
       <c r="J91" t="s">
@@ -1657,11 +2080,11 @@
     </row>
     <row r="92" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H92">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2.1843886419491501</v>
       </c>
       <c r="I92">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>179</v>
       </c>
       <c r="J92" t="s">
@@ -1670,11 +2093,11 @@
     </row>
     <row r="93" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H93">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2.2089323345553202</v>
       </c>
       <c r="I93">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>178</v>
       </c>
       <c r="J93" t="s">
@@ -1683,11 +2106,11 @@
     </row>
     <row r="94" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H94">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2.2334760271614904</v>
       </c>
       <c r="I94">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>177</v>
       </c>
       <c r="J94" t="s">
@@ -1696,11 +2119,11 @@
     </row>
     <row r="95" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H95">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2.2580197197676606</v>
       </c>
       <c r="I95">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>176</v>
       </c>
       <c r="J95" t="s">
@@ -1709,11 +2132,11 @@
     </row>
     <row r="96" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H96">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2.2825634123738308</v>
       </c>
       <c r="I96">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>175</v>
       </c>
       <c r="J96" t="s">
@@ -1722,11 +2145,11 @@
     </row>
     <row r="97" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H97">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2.3071071049800009</v>
       </c>
       <c r="I97">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>174</v>
       </c>
       <c r="J97" t="s">
@@ -1735,11 +2158,11 @@
     </row>
     <row r="98" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H98">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2.3316507975861711</v>
       </c>
       <c r="I98">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>173</v>
       </c>
       <c r="J98" t="s">
@@ -1748,11 +2171,11 @@
     </row>
     <row r="99" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H99">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2.3561944901923413</v>
       </c>
       <c r="I99">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>172</v>
       </c>
       <c r="J99" t="s">
@@ -1761,11 +2184,11 @@
     </row>
     <row r="100" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H100">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2.3807381827985115</v>
       </c>
       <c r="I100">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>171</v>
       </c>
       <c r="J100" t="s">
@@ -1774,11 +2197,11 @@
     </row>
     <row r="101" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H101">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2.4052818754046816</v>
       </c>
       <c r="I101">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>170</v>
       </c>
       <c r="J101" t="s">
@@ -1787,11 +2210,11 @@
     </row>
     <row r="102" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H102">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2.4298255680108518</v>
       </c>
       <c r="I102">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>169</v>
       </c>
       <c r="J102" t="s">
@@ -1800,11 +2223,11 @@
     </row>
     <row r="103" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H103">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2.454369260617022</v>
       </c>
       <c r="I103">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>168</v>
       </c>
       <c r="J103" t="s">
@@ -1813,11 +2236,11 @@
     </row>
     <row r="104" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H104">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2.4789129532231922</v>
       </c>
       <c r="I104">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>166</v>
       </c>
       <c r="J104" t="s">
@@ -1826,11 +2249,11 @@
     </row>
     <row r="105" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H105">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2.5034566458293623</v>
       </c>
       <c r="I105">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>165</v>
       </c>
       <c r="J105" t="s">
@@ -1839,11 +2262,11 @@
     </row>
     <row r="106" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H106">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2.5280003384355325</v>
       </c>
       <c r="I106">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>164</v>
       </c>
       <c r="J106" t="s">
@@ -1852,11 +2275,11 @@
     </row>
     <row r="107" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H107">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2.5525440310417027</v>
       </c>
       <c r="I107">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>163</v>
       </c>
       <c r="J107" t="s">
@@ -1865,11 +2288,11 @@
     </row>
     <row r="108" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H108">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2.5770877236478729</v>
       </c>
       <c r="I108">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>161</v>
       </c>
       <c r="J108" t="s">
@@ -1878,11 +2301,11 @@
     </row>
     <row r="109" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H109">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2.601631416254043</v>
       </c>
       <c r="I109">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>160</v>
       </c>
       <c r="J109" t="s">
@@ -1891,11 +2314,11 @@
     </row>
     <row r="110" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H110">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2.6261751088602132</v>
       </c>
       <c r="I110">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>159</v>
       </c>
       <c r="J110" t="s">
@@ -1904,11 +2327,11 @@
     </row>
     <row r="111" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H111">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2.6507188014663834</v>
       </c>
       <c r="I111">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>157</v>
       </c>
       <c r="J111" t="s">
@@ -1917,11 +2340,11 @@
     </row>
     <row r="112" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H112">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2.6752624940725536</v>
       </c>
       <c r="I112">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>156</v>
       </c>
       <c r="J112" t="s">
@@ -1930,11 +2353,11 @@
     </row>
     <row r="113" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H113">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2.6998061866787237</v>
       </c>
       <c r="I113">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>154</v>
       </c>
       <c r="J113" t="s">
@@ -1943,11 +2366,11 @@
     </row>
     <row r="114" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H114">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2.7243498792848939</v>
       </c>
       <c r="I114">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>153</v>
       </c>
       <c r="J114" t="s">
@@ -1956,11 +2379,11 @@
     </row>
     <row r="115" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H115">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2.7488935718910641</v>
       </c>
       <c r="I115">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>151</v>
       </c>
       <c r="J115" t="s">
@@ -1969,11 +2392,11 @@
     </row>
     <row r="116" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H116">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2.7734372644972343</v>
       </c>
       <c r="I116">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>150</v>
       </c>
       <c r="J116" t="s">
@@ -1982,11 +2405,11 @@
     </row>
     <row r="117" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H117">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2.7979809571034044</v>
       </c>
       <c r="I117">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>149</v>
       </c>
       <c r="J117" t="s">
@@ -1995,11 +2418,11 @@
     </row>
     <row r="118" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H118">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2.8225246497095746</v>
       </c>
       <c r="I118">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>147</v>
       </c>
       <c r="J118" t="s">
@@ -2008,11 +2431,11 @@
     </row>
     <row r="119" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H119">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2.8470683423157448</v>
       </c>
       <c r="I119">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>146</v>
       </c>
       <c r="J119" t="s">
@@ -2021,11 +2444,11 @@
     </row>
     <row r="120" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H120">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2.871612034921915</v>
       </c>
       <c r="I120">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>144</v>
       </c>
       <c r="J120" t="s">
@@ -2034,11 +2457,11 @@
     </row>
     <row r="121" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H121">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2.8961557275280851</v>
       </c>
       <c r="I121">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>143</v>
       </c>
       <c r="J121" t="s">
@@ -2047,11 +2470,11 @@
     </row>
     <row r="122" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H122">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2.9206994201342553</v>
       </c>
       <c r="I122">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>141</v>
       </c>
       <c r="J122" t="s">
@@ -2060,11 +2483,11 @@
     </row>
     <row r="123" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H123">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2.9452431127404255</v>
       </c>
       <c r="I123">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>139</v>
       </c>
       <c r="J123" t="s">
@@ -2073,11 +2496,11 @@
     </row>
     <row r="124" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H124">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2.9697868053465957</v>
       </c>
       <c r="I124">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>138</v>
       </c>
       <c r="J124" t="s">
@@ -2086,11 +2509,11 @@
     </row>
     <row r="125" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H125">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2.9943304979527658</v>
       </c>
       <c r="I125">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>136</v>
       </c>
       <c r="J125" t="s">
@@ -2099,11 +2522,11 @@
     </row>
     <row r="126" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H126">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>3.018874190558936</v>
       </c>
       <c r="I126">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>135</v>
       </c>
       <c r="J126" t="s">
@@ -2112,11 +2535,11 @@
     </row>
     <row r="127" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H127">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>3.0434178831651062</v>
       </c>
       <c r="I127">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>133</v>
       </c>
       <c r="J127" t="s">
@@ -2125,11 +2548,11 @@
     </row>
     <row r="128" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H128">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>3.0679615757712764</v>
       </c>
       <c r="I128">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>132</v>
       </c>
       <c r="J128" t="s">
@@ -2138,11 +2561,11 @@
     </row>
     <row r="129" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H129">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>3.0925052683774465</v>
       </c>
       <c r="I129">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>130</v>
       </c>
       <c r="J129" t="s">
@@ -2151,11 +2574,11 @@
     </row>
     <row r="130" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H130">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>3.1170489609836167</v>
       </c>
       <c r="I130">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>129</v>
       </c>
       <c r="J130" t="s">
@@ -2164,11 +2587,11 @@
     </row>
     <row r="131" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H131">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>3.1415926535897869</v>
       </c>
       <c r="I131">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>127</v>
       </c>
       <c r="J131" t="s">
@@ -2177,11 +2600,11 @@
     </row>
     <row r="132" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H132">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>3.1661363461959571</v>
       </c>
       <c r="I132">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>125</v>
       </c>
       <c r="J132" t="s">
@@ -2190,11 +2613,11 @@
     </row>
     <row r="133" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H133">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>3.1906800388021272</v>
       </c>
       <c r="I133">
-        <f t="shared" ref="I133:I196" si="4">ROUND(SIN(H133)*64+127,0)</f>
+        <f t="shared" ref="I133:I196" si="8">ROUND(SIN(H133)*64+127,0)</f>
         <v>124</v>
       </c>
       <c r="J133" t="s">
@@ -2203,11 +2626,11 @@
     </row>
     <row r="134" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H134">
-        <f t="shared" ref="H134:H197" si="5">H133+$I$2</f>
+        <f t="shared" ref="H134:H197" si="9">H133+$I$2</f>
         <v>3.2152237314082974</v>
       </c>
       <c r="I134">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>122</v>
       </c>
       <c r="J134" t="s">
@@ -2216,11 +2639,11 @@
     </row>
     <row r="135" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H135">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>3.2397674240144676</v>
       </c>
       <c r="I135">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>121</v>
       </c>
       <c r="J135" t="s">
@@ -2229,11 +2652,11 @@
     </row>
     <row r="136" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H136">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>3.2643111166206378</v>
       </c>
       <c r="I136">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>119</v>
       </c>
       <c r="J136" t="s">
@@ -2242,11 +2665,11 @@
     </row>
     <row r="137" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H137">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>3.288854809226808</v>
       </c>
       <c r="I137">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>118</v>
       </c>
       <c r="J137" t="s">
@@ -2255,11 +2678,11 @@
     </row>
     <row r="138" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H138">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>3.3133985018329781</v>
       </c>
       <c r="I138">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>116</v>
       </c>
       <c r="J138" t="s">
@@ -2268,11 +2691,11 @@
     </row>
     <row r="139" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H139">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>3.3379421944391483</v>
       </c>
       <c r="I139">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>115</v>
       </c>
       <c r="J139" t="s">
@@ -2281,11 +2704,11 @@
     </row>
     <row r="140" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H140">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>3.3624858870453185</v>
       </c>
       <c r="I140">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>113</v>
       </c>
       <c r="J140" t="s">
@@ -2294,11 +2717,11 @@
     </row>
     <row r="141" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H141">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>3.3870295796514887</v>
       </c>
       <c r="I141">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>111</v>
       </c>
       <c r="J141" t="s">
@@ -2307,11 +2730,11 @@
     </row>
     <row r="142" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H142">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>3.4115732722576588</v>
       </c>
       <c r="I142">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>110</v>
       </c>
       <c r="J142" t="s">
@@ -2320,11 +2743,11 @@
     </row>
     <row r="143" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H143">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>3.436116964863829</v>
       </c>
       <c r="I143">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>108</v>
       </c>
       <c r="J143" t="s">
@@ -2333,11 +2756,11 @@
     </row>
     <row r="144" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H144">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>3.4606606574699992</v>
       </c>
       <c r="I144">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>107</v>
       </c>
       <c r="J144" t="s">
@@ -2346,11 +2769,11 @@
     </row>
     <row r="145" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H145">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>3.4852043500761694</v>
       </c>
       <c r="I145">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>105</v>
       </c>
       <c r="J145" t="s">
@@ -2359,11 +2782,11 @@
     </row>
     <row r="146" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H146">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>3.5097480426823395</v>
       </c>
       <c r="I146">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>104</v>
       </c>
       <c r="J146" t="s">
@@ -2372,11 +2795,11 @@
     </row>
     <row r="147" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H147">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>3.5342917352885097</v>
       </c>
       <c r="I147">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>103</v>
       </c>
       <c r="J147" t="s">
@@ -2385,11 +2808,11 @@
     </row>
     <row r="148" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H148">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>3.5588354278946799</v>
       </c>
       <c r="I148">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>101</v>
       </c>
       <c r="J148" t="s">
@@ -2398,11 +2821,11 @@
     </row>
     <row r="149" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H149">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>3.5833791205008501</v>
       </c>
       <c r="I149">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>100</v>
       </c>
       <c r="J149" t="s">
@@ -2411,11 +2834,11 @@
     </row>
     <row r="150" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H150">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>3.6079228131070202</v>
       </c>
       <c r="I150">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>98</v>
       </c>
       <c r="J150" t="s">
@@ -2424,11 +2847,11 @@
     </row>
     <row r="151" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H151">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>3.6324665057131904</v>
       </c>
       <c r="I151">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>97</v>
       </c>
       <c r="J151" t="s">
@@ -2437,11 +2860,11 @@
     </row>
     <row r="152" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H152">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>3.6570101983193606</v>
       </c>
       <c r="I152">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>95</v>
       </c>
       <c r="J152" t="s">
@@ -2450,11 +2873,11 @@
     </row>
     <row r="153" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H153">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>3.6815538909255308</v>
       </c>
       <c r="I153">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>94</v>
       </c>
       <c r="J153" t="s">
@@ -2463,11 +2886,11 @@
     </row>
     <row r="154" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H154">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>3.7060975835317009</v>
       </c>
       <c r="I154">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>93</v>
       </c>
       <c r="J154" t="s">
@@ -2476,11 +2899,11 @@
     </row>
     <row r="155" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H155">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>3.7306412761378711</v>
       </c>
       <c r="I155">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>91</v>
       </c>
       <c r="J155" t="s">
@@ -2489,11 +2912,11 @@
     </row>
     <row r="156" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H156">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>3.7551849687440413</v>
       </c>
       <c r="I156">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>90</v>
       </c>
       <c r="J156" t="s">
@@ -2502,11 +2925,11 @@
     </row>
     <row r="157" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H157">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>3.7797286613502115</v>
       </c>
       <c r="I157">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>89</v>
       </c>
       <c r="J157" t="s">
@@ -2515,11 +2938,11 @@
     </row>
     <row r="158" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H158">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>3.8042723539563816</v>
       </c>
       <c r="I158">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>88</v>
       </c>
       <c r="J158" t="s">
@@ -2528,11 +2951,11 @@
     </row>
     <row r="159" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H159">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>3.8288160465625518</v>
       </c>
       <c r="I159">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>86</v>
       </c>
       <c r="J159" t="s">
@@ -2541,11 +2964,11 @@
     </row>
     <row r="160" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H160">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>3.853359739168722</v>
       </c>
       <c r="I160">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>85</v>
       </c>
       <c r="J160" t="s">
@@ -2554,11 +2977,11 @@
     </row>
     <row r="161" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H161">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>3.8779034317748922</v>
       </c>
       <c r="I161">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>84</v>
       </c>
       <c r="J161" t="s">
@@ -2567,11 +2990,11 @@
     </row>
     <row r="162" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H162">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>3.9024471243810623</v>
       </c>
       <c r="I162">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>83</v>
       </c>
       <c r="J162" t="s">
@@ -2580,11 +3003,11 @@
     </row>
     <row r="163" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H163">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>3.9269908169872325</v>
       </c>
       <c r="I163">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>82</v>
       </c>
       <c r="J163" t="s">
@@ -2593,11 +3016,11 @@
     </row>
     <row r="164" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H164">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>3.9515345095934027</v>
       </c>
       <c r="I164">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>81</v>
       </c>
       <c r="J164" t="s">
@@ -2606,11 +3029,11 @@
     </row>
     <row r="165" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H165">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>3.9760782021995729</v>
       </c>
       <c r="I165">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>80</v>
       </c>
       <c r="J165" t="s">
@@ -2619,11 +3042,11 @@
     </row>
     <row r="166" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H166">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>4.000621894805743</v>
       </c>
       <c r="I166">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>79</v>
       </c>
       <c r="J166" t="s">
@@ -2632,11 +3055,11 @@
     </row>
     <row r="167" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H167">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>4.0251655874119132</v>
       </c>
       <c r="I167">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>78</v>
       </c>
       <c r="J167" t="s">
@@ -2645,11 +3068,11 @@
     </row>
     <row r="168" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H168">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>4.0497092800180834</v>
       </c>
       <c r="I168">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>77</v>
       </c>
       <c r="J168" t="s">
@@ -2658,11 +3081,11 @@
     </row>
     <row r="169" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H169">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>4.0742529726242536</v>
       </c>
       <c r="I169">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>76</v>
       </c>
       <c r="J169" t="s">
@@ -2671,11 +3094,11 @@
     </row>
     <row r="170" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H170">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>4.0987966652304237</v>
       </c>
       <c r="I170">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>75</v>
       </c>
       <c r="J170" t="s">
@@ -2684,11 +3107,11 @@
     </row>
     <row r="171" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H171">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>4.1233403578365939</v>
       </c>
       <c r="I171">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>74</v>
       </c>
       <c r="J171" t="s">
@@ -2697,11 +3120,11 @@
     </row>
     <row r="172" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H172">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>4.1478840504427641</v>
       </c>
       <c r="I172">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>73</v>
       </c>
       <c r="J172" t="s">
@@ -2710,11 +3133,11 @@
     </row>
     <row r="173" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H173">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>4.1724277430489343</v>
       </c>
       <c r="I173">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>72</v>
       </c>
       <c r="J173" t="s">
@@ -2723,11 +3146,11 @@
     </row>
     <row r="174" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H174">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>4.1969714356551044</v>
       </c>
       <c r="I174">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>71</v>
       </c>
       <c r="J174" t="s">
@@ -2736,11 +3159,11 @@
     </row>
     <row r="175" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H175">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>4.2215151282612746</v>
       </c>
       <c r="I175">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>71</v>
       </c>
       <c r="J175" t="s">
@@ -2749,11 +3172,11 @@
     </row>
     <row r="176" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H176">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>4.2460588208674448</v>
       </c>
       <c r="I176">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>70</v>
       </c>
       <c r="J176" t="s">
@@ -2762,11 +3185,11 @@
     </row>
     <row r="177" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H177">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>4.270602513473615</v>
       </c>
       <c r="I177">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>69</v>
       </c>
       <c r="J177" t="s">
@@ -2775,11 +3198,11 @@
     </row>
     <row r="178" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H178">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>4.2951462060797851</v>
       </c>
       <c r="I178">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>68</v>
       </c>
       <c r="J178" t="s">
@@ -2788,11 +3211,11 @@
     </row>
     <row r="179" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H179">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>4.3196898986859553</v>
       </c>
       <c r="I179">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>68</v>
       </c>
       <c r="J179" t="s">
@@ -2801,11 +3224,11 @@
     </row>
     <row r="180" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H180">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>4.3442335912921255</v>
       </c>
       <c r="I180">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>67</v>
       </c>
       <c r="J180" t="s">
@@ -2814,11 +3237,11 @@
     </row>
     <row r="181" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H181">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>4.3687772838982957</v>
       </c>
       <c r="I181">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>67</v>
       </c>
       <c r="J181" t="s">
@@ -2827,11 +3250,11 @@
     </row>
     <row r="182" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H182">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>4.3933209765044658</v>
       </c>
       <c r="I182">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>66</v>
       </c>
       <c r="J182" t="s">
@@ -2840,11 +3263,11 @@
     </row>
     <row r="183" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H183">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>4.417864669110636</v>
       </c>
       <c r="I183">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>66</v>
       </c>
       <c r="J183" t="s">
@@ -2853,11 +3276,11 @@
     </row>
     <row r="184" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H184">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>4.4424083617168062</v>
       </c>
       <c r="I184">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>65</v>
       </c>
       <c r="J184" t="s">
@@ -2866,11 +3289,11 @@
     </row>
     <row r="185" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H185">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>4.4669520543229764</v>
       </c>
       <c r="I185">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>65</v>
       </c>
       <c r="J185" t="s">
@@ -2879,11 +3302,11 @@
     </row>
     <row r="186" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H186">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>4.4914957469291465</v>
       </c>
       <c r="I186">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>65</v>
       </c>
       <c r="J186" t="s">
@@ -2892,11 +3315,11 @@
     </row>
     <row r="187" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H187">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>4.5160394395353167</v>
       </c>
       <c r="I187">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>64</v>
       </c>
       <c r="J187" t="s">
@@ -2905,11 +3328,11 @@
     </row>
     <row r="188" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H188">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>4.5405831321414869</v>
       </c>
       <c r="I188">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>64</v>
       </c>
       <c r="J188" t="s">
@@ -2918,11 +3341,11 @@
     </row>
     <row r="189" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H189">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>4.5651268247476571</v>
       </c>
       <c r="I189">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>64</v>
       </c>
       <c r="J189" t="s">
@@ -2931,11 +3354,11 @@
     </row>
     <row r="190" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H190">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>4.5896705173538273</v>
       </c>
       <c r="I190">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>63</v>
       </c>
       <c r="J190" t="s">
@@ -2944,11 +3367,11 @@
     </row>
     <row r="191" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H191">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>4.6142142099599974</v>
       </c>
       <c r="I191">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>63</v>
       </c>
       <c r="J191" t="s">
@@ -2957,11 +3380,11 @@
     </row>
     <row r="192" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H192">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>4.6387579025661676</v>
       </c>
       <c r="I192">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>63</v>
       </c>
       <c r="J192" t="s">
@@ -2970,11 +3393,11 @@
     </row>
     <row r="193" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H193">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>4.6633015951723378</v>
       </c>
       <c r="I193">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>63</v>
       </c>
       <c r="J193" t="s">
@@ -2983,11 +3406,11 @@
     </row>
     <row r="194" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H194">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>4.687845287778508</v>
       </c>
       <c r="I194">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>63</v>
       </c>
       <c r="J194" t="s">
@@ -2996,11 +3419,11 @@
     </row>
     <row r="195" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H195">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>4.7123889803846781</v>
       </c>
       <c r="I195">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>63</v>
       </c>
       <c r="J195" t="s">
@@ -3009,11 +3432,11 @@
     </row>
     <row r="196" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H196">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>4.7369326729908483</v>
       </c>
       <c r="I196">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>63</v>
       </c>
       <c r="J196" t="s">
@@ -3022,11 +3445,11 @@
     </row>
     <row r="197" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H197">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>4.7614763655970185</v>
       </c>
       <c r="I197">
-        <f t="shared" ref="I197:I259" si="6">ROUND(SIN(H197)*64+127,0)</f>
+        <f t="shared" ref="I197:I259" si="10">ROUND(SIN(H197)*64+127,0)</f>
         <v>63</v>
       </c>
       <c r="J197" t="s">
@@ -3035,11 +3458,11 @@
     </row>
     <row r="198" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H198">
-        <f t="shared" ref="H198:H261" si="7">H197+$I$2</f>
+        <f t="shared" ref="H198:H259" si="11">H197+$I$2</f>
         <v>4.7860200582031887</v>
       </c>
       <c r="I198">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>63</v>
       </c>
       <c r="J198" t="s">
@@ -3048,11 +3471,11 @@
     </row>
     <row r="199" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H199">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>4.8105637508093588</v>
       </c>
       <c r="I199">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>63</v>
       </c>
       <c r="J199" t="s">
@@ -3061,11 +3484,11 @@
     </row>
     <row r="200" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H200">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>4.835107443415529</v>
       </c>
       <c r="I200">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>63</v>
       </c>
       <c r="J200" t="s">
@@ -3074,11 +3497,11 @@
     </row>
     <row r="201" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H201">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>4.8596511360216992</v>
       </c>
       <c r="I201">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>64</v>
       </c>
       <c r="J201" t="s">
@@ -3087,11 +3510,11 @@
     </row>
     <row r="202" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H202">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>4.8841948286278694</v>
       </c>
       <c r="I202">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>64</v>
       </c>
       <c r="J202" t="s">
@@ -3100,11 +3523,11 @@
     </row>
     <row r="203" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H203">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>4.9087385212340395</v>
       </c>
       <c r="I203">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>64</v>
       </c>
       <c r="J203" t="s">
@@ -3113,11 +3536,11 @@
     </row>
     <row r="204" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H204">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>4.9332822138402097</v>
       </c>
       <c r="I204">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>65</v>
       </c>
       <c r="J204" t="s">
@@ -3126,11 +3549,11 @@
     </row>
     <row r="205" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H205">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>4.9578259064463799</v>
       </c>
       <c r="I205">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>65</v>
       </c>
       <c r="J205" t="s">
@@ -3139,11 +3562,11 @@
     </row>
     <row r="206" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H206">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>4.9823695990525501</v>
       </c>
       <c r="I206">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>65</v>
       </c>
       <c r="J206" t="s">
@@ -3152,11 +3575,11 @@
     </row>
     <row r="207" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H207">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>5.0069132916587202</v>
       </c>
       <c r="I207">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>66</v>
       </c>
       <c r="J207" t="s">
@@ -3165,11 +3588,11 @@
     </row>
     <row r="208" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H208">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>5.0314569842648904</v>
       </c>
       <c r="I208">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>66</v>
       </c>
       <c r="J208" t="s">
@@ -3178,11 +3601,11 @@
     </row>
     <row r="209" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H209">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>5.0560006768710606</v>
       </c>
       <c r="I209">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>67</v>
       </c>
       <c r="J209" t="s">
@@ -3191,11 +3614,11 @@
     </row>
     <row r="210" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H210">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>5.0805443694772308</v>
       </c>
       <c r="I210">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>67</v>
       </c>
       <c r="J210" t="s">
@@ -3204,11 +3627,11 @@
     </row>
     <row r="211" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H211">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>5.1050880620834009</v>
       </c>
       <c r="I211">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>68</v>
       </c>
       <c r="J211" t="s">
@@ -3217,11 +3640,11 @@
     </row>
     <row r="212" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H212">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>5.1296317546895711</v>
       </c>
       <c r="I212">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>68</v>
       </c>
       <c r="J212" t="s">
@@ -3230,11 +3653,11 @@
     </row>
     <row r="213" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H213">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>5.1541754472957413</v>
       </c>
       <c r="I213">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>69</v>
       </c>
       <c r="J213" t="s">
@@ -3243,11 +3666,11 @@
     </row>
     <row r="214" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H214">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>5.1787191399019115</v>
       </c>
       <c r="I214">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>70</v>
       </c>
       <c r="J214" t="s">
@@ -3256,11 +3679,11 @@
     </row>
     <row r="215" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H215">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>5.2032628325080816</v>
       </c>
       <c r="I215">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>71</v>
       </c>
       <c r="J215" t="s">
@@ -3269,11 +3692,11 @@
     </row>
     <row r="216" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H216">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>5.2278065251142518</v>
       </c>
       <c r="I216">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>71</v>
       </c>
       <c r="J216" t="s">
@@ -3282,11 +3705,11 @@
     </row>
     <row r="217" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H217">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>5.252350217720422</v>
       </c>
       <c r="I217">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>72</v>
       </c>
       <c r="J217" t="s">
@@ -3295,11 +3718,11 @@
     </row>
     <row r="218" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H218">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>5.2768939103265922</v>
       </c>
       <c r="I218">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>73</v>
       </c>
       <c r="J218" t="s">
@@ -3308,11 +3731,11 @@
     </row>
     <row r="219" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H219">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>5.3014376029327623</v>
       </c>
       <c r="I219">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>74</v>
       </c>
       <c r="J219" t="s">
@@ -3321,11 +3744,11 @@
     </row>
     <row r="220" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H220">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>5.3259812955389325</v>
       </c>
       <c r="I220">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>75</v>
       </c>
       <c r="J220" t="s">
@@ -3334,11 +3757,11 @@
     </row>
     <row r="221" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H221">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>5.3505249881451027</v>
       </c>
       <c r="I221">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>76</v>
       </c>
       <c r="J221" t="s">
@@ -3347,11 +3770,11 @@
     </row>
     <row r="222" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H222">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>5.3750686807512729</v>
       </c>
       <c r="I222">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>77</v>
       </c>
       <c r="J222" t="s">
@@ -3360,11 +3783,11 @@
     </row>
     <row r="223" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H223">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>5.399612373357443</v>
       </c>
       <c r="I223">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>78</v>
       </c>
       <c r="J223" t="s">
@@ -3373,11 +3796,11 @@
     </row>
     <row r="224" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H224">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>5.4241560659636132</v>
       </c>
       <c r="I224">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>79</v>
       </c>
       <c r="J224" t="s">
@@ -3386,11 +3809,11 @@
     </row>
     <row r="225" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H225">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>5.4486997585697834</v>
       </c>
       <c r="I225">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>80</v>
       </c>
       <c r="J225" t="s">
@@ -3399,11 +3822,11 @@
     </row>
     <row r="226" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H226">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>5.4732434511759536</v>
       </c>
       <c r="I226">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>81</v>
       </c>
       <c r="J226" t="s">
@@ -3412,11 +3835,11 @@
     </row>
     <row r="227" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H227">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>5.4977871437821237</v>
       </c>
       <c r="I227">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>82</v>
       </c>
       <c r="J227" t="s">
@@ -3425,11 +3848,11 @@
     </row>
     <row r="228" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H228">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>5.5223308363882939</v>
       </c>
       <c r="I228">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>83</v>
       </c>
       <c r="J228" t="s">
@@ -3438,11 +3861,11 @@
     </row>
     <row r="229" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H229">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>5.5468745289944641</v>
       </c>
       <c r="I229">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>84</v>
       </c>
       <c r="J229" t="s">
@@ -3451,11 +3874,11 @@
     </row>
     <row r="230" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H230">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>5.5714182216006343</v>
       </c>
       <c r="I230">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>85</v>
       </c>
       <c r="J230" t="s">
@@ -3464,11 +3887,11 @@
     </row>
     <row r="231" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H231">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>5.5959619142068044</v>
       </c>
       <c r="I231">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>86</v>
       </c>
       <c r="J231" t="s">
@@ -3477,11 +3900,11 @@
     </row>
     <row r="232" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H232">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>5.6205056068129746</v>
       </c>
       <c r="I232">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>88</v>
       </c>
       <c r="J232" t="s">
@@ -3490,11 +3913,11 @@
     </row>
     <row r="233" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H233">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>5.6450492994191448</v>
       </c>
       <c r="I233">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>89</v>
       </c>
       <c r="J233" t="s">
@@ -3503,11 +3926,11 @@
     </row>
     <row r="234" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H234">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>5.669592992025315</v>
       </c>
       <c r="I234">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>90</v>
       </c>
       <c r="J234" t="s">
@@ -3516,11 +3939,11 @@
     </row>
     <row r="235" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H235">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>5.6941366846314851</v>
       </c>
       <c r="I235">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>91</v>
       </c>
       <c r="J235" t="s">
@@ -3529,11 +3952,11 @@
     </row>
     <row r="236" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H236">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>5.7186803772376553</v>
       </c>
       <c r="I236">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>93</v>
       </c>
       <c r="J236" t="s">
@@ -3542,11 +3965,11 @@
     </row>
     <row r="237" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H237">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>5.7432240698438255</v>
       </c>
       <c r="I237">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>94</v>
       </c>
       <c r="J237" t="s">
@@ -3555,11 +3978,11 @@
     </row>
     <row r="238" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H238">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>5.7677677624499957</v>
       </c>
       <c r="I238">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>95</v>
       </c>
       <c r="J238" t="s">
@@ -3568,11 +3991,11 @@
     </row>
     <row r="239" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H239">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>5.7923114550561658</v>
       </c>
       <c r="I239">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>97</v>
       </c>
       <c r="J239" t="s">
@@ -3581,11 +4004,11 @@
     </row>
     <row r="240" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H240">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>5.816855147662336</v>
       </c>
       <c r="I240">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>98</v>
       </c>
       <c r="J240" t="s">
@@ -3594,11 +4017,11 @@
     </row>
     <row r="241" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H241">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>5.8413988402685062</v>
       </c>
       <c r="I241">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>100</v>
       </c>
       <c r="J241" t="s">
@@ -3607,11 +4030,11 @@
     </row>
     <row r="242" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H242">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>5.8659425328746764</v>
       </c>
       <c r="I242">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>101</v>
       </c>
       <c r="J242" t="s">
@@ -3620,11 +4043,11 @@
     </row>
     <row r="243" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H243">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>5.8904862254808465</v>
       </c>
       <c r="I243">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>103</v>
       </c>
       <c r="J243" t="s">
@@ -3633,11 +4056,11 @@
     </row>
     <row r="244" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H244">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>5.9150299180870167</v>
       </c>
       <c r="I244">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>104</v>
       </c>
       <c r="J244" t="s">
@@ -3646,11 +4069,11 @@
     </row>
     <row r="245" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H245">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>5.9395736106931869</v>
       </c>
       <c r="I245">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>105</v>
       </c>
       <c r="J245" t="s">
@@ -3659,11 +4082,11 @@
     </row>
     <row r="246" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H246">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>5.9641173032993571</v>
       </c>
       <c r="I246">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>107</v>
       </c>
       <c r="J246" t="s">
@@ -3672,11 +4095,11 @@
     </row>
     <row r="247" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H247">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>5.9886609959055273</v>
       </c>
       <c r="I247">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>108</v>
       </c>
       <c r="J247" t="s">
@@ -3685,11 +4108,11 @@
     </row>
     <row r="248" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H248">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>6.0132046885116974</v>
       </c>
       <c r="I248">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>110</v>
       </c>
       <c r="J248" t="s">
@@ -3698,11 +4121,11 @@
     </row>
     <row r="249" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H249">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>6.0377483811178676</v>
       </c>
       <c r="I249">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>111</v>
       </c>
       <c r="J249" t="s">
@@ -3711,11 +4134,11 @@
     </row>
     <row r="250" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H250">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>6.0622920737240378</v>
       </c>
       <c r="I250">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>113</v>
       </c>
       <c r="J250" t="s">
@@ -3724,11 +4147,11 @@
     </row>
     <row r="251" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H251">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>6.086835766330208</v>
       </c>
       <c r="I251">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>115</v>
       </c>
       <c r="J251" t="s">
@@ -3737,11 +4160,11 @@
     </row>
     <row r="252" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H252">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>6.1113794589363781</v>
       </c>
       <c r="I252">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>116</v>
       </c>
       <c r="J252" t="s">
@@ -3750,11 +4173,11 @@
     </row>
     <row r="253" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H253">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>6.1359231515425483</v>
       </c>
       <c r="I253">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>118</v>
       </c>
       <c r="J253" t="s">
@@ -3763,11 +4186,11 @@
     </row>
     <row r="254" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H254">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>6.1604668441487185</v>
       </c>
       <c r="I254">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>119</v>
       </c>
       <c r="J254" t="s">
@@ -3776,11 +4199,11 @@
     </row>
     <row r="255" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H255">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>6.1850105367548887</v>
       </c>
       <c r="I255">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>121</v>
       </c>
       <c r="J255" t="s">
@@ -3789,11 +4212,11 @@
     </row>
     <row r="256" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H256">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>6.2095542293610588</v>
       </c>
       <c r="I256">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>122</v>
       </c>
       <c r="J256" t="s">
@@ -3802,11 +4225,11 @@
     </row>
     <row r="257" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H257">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>6.234097921967229</v>
       </c>
       <c r="I257">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>124</v>
       </c>
       <c r="J257" t="s">
@@ -3815,11 +4238,11 @@
     </row>
     <row r="258" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H258">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>6.2586416145733992</v>
       </c>
       <c r="I258">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>125</v>
       </c>
       <c r="J258" t="s">
@@ -3828,15 +4251,22 @@
     </row>
     <row r="259" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H259">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>6.2831853071795694</v>
       </c>
       <c r="I259">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>127</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="D9:G9"/>
+    <mergeCell ref="D19:G19"/>
+    <mergeCell ref="D7:G8"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>